<commit_message>
fix(passenger/index.css): download passenger Template/index.css
</commit_message>
<xml_diff>
--- a/public/passengerTemplate.xlsx
+++ b/public/passengerTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16200"/>
+    <workbookView windowHeight="24320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -55,10 +55,7 @@
     <t>mrs</t>
   </si>
   <si>
-    <t>HU</t>
-  </si>
-  <si>
-    <t>JUN</t>
+    <t>TEST</t>
   </si>
   <si>
     <t>male</t>
@@ -88,10 +85,13 @@
     <t>INF</t>
   </si>
   <si>
+    <t>mr</t>
+  </si>
+  <si>
     <t>miss</t>
   </si>
   <si>
-    <t>mstr</t>
+    <t>mastr</t>
   </si>
 </sst>
 </file>
@@ -99,12 +99,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -113,18 +113,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -132,6 +134,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -146,8 +156,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,17 +195,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,7 +220,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,9 +235,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -208,16 +248,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,44 +258,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,187 +272,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,6 +475,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -492,15 +504,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,15 +523,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -540,17 +534,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,157 +552,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1042,7 +1036,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6"/>
@@ -1101,48 +1095,48 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>